<commit_message>
Lecture du tableau panier pour son affichage ; mise à jour d'un aticle (prix et qte) avec les boutons +/- dans le panier ; Lecture du tableau livres et affichage des Cards dans la page
</commit_message>
<xml_diff>
--- a/WORK/Livres.xlsx
+++ b/WORK/Livres.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20010" windowHeight="12180" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20010" windowHeight="12180"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I45" sqref="G1:I45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,19 +1075,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I45" sqref="G1:I45"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="str">
         <f>CONCATENATE("&lt;livre id=""",A1,"""&gt;")</f>
-        <v>&lt;livre id="5"&gt;</v>
+        <v>&lt;livre id="6"&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1131,8 +1131,8 @@
         <v>12</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A6),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2372509-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A6),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2372509-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1140,8 +1140,8 @@
         <v>13</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A7),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Sciences&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A7),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1161,11 +1161,11 @@
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A1+1</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE("&lt;livre id=""",A10,"""&gt;")</f>
-        <v>&lt;livre id="6"&gt;</v>
+        <v>&lt;livre id="7"&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1209,8 +1209,8 @@
         <v>15</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A15),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2385277-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A15),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2385277-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1218,8 +1218,8 @@
         <v>13</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A16),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Sciences&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1239,11 +1239,11 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A10+1</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE("&lt;livre id=""",A19,"""&gt;")</f>
-        <v>&lt;livre id="7"&gt;</v>
+        <v>&lt;livre id="8"&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1287,8 +1287,8 @@
         <v>17</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A24),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2420464-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A24),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2420464-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1296,8 +1296,8 @@
         <v>13</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A25),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Sciences&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1317,11 +1317,11 @@
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A19+1</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H28" t="str">
         <f>CONCATENATE("&lt;livre id=""",A28,"""&gt;")</f>
-        <v>&lt;livre id="8"&gt;</v>
+        <v>&lt;livre id="9"&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1365,8 +1365,8 @@
         <v>19</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A33),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2425434-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A33),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2425434-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1374,8 +1374,8 @@
         <v>13</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A34),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Sciences&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1395,11 +1395,11 @@
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A28+1</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("&lt;livre id=""",A37,"""&gt;")</f>
-        <v>&lt;livre id="9"&gt;</v>
+        <v>&lt;livre id="10"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1443,8 +1443,8 @@
         <v>22</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A42),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2386203-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A42),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2386203-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1452,8 +1452,8 @@
         <v>13</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A43),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Sciences&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1480,7 +1480,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I45" sqref="G1:I45"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,8 +1535,8 @@
         <v>24</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A6),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2373231-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A6),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2373231-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1544,8 +1544,8 @@
         <v>44</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A7),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Histoire&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A7),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1613,8 +1613,8 @@
         <v>26</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A15),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2428907-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A15),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2428907-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1622,8 +1622,8 @@
         <v>44</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A16),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Histoire&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1691,8 +1691,8 @@
         <v>28</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A24),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2443637-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A24),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2443637-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1700,8 +1700,8 @@
         <v>44</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A25),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Histoire&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1769,8 +1769,8 @@
         <v>30</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A33),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2372375-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A33),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2372375-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -1778,8 +1778,8 @@
         <v>44</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A34),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Histoire&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -1847,8 +1847,8 @@
         <v>32</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A42),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2432344-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A42),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2432344-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -1856,8 +1856,8 @@
         <v>44</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A43),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Histoire&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -1884,7 +1884,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15:I16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1939,8 +1939,8 @@
         <v>34</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A6),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2293868-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A6),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2293868-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1948,8 +1948,8 @@
         <v>103</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A7),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;BD &amp;amp; Mangas&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A7),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2017,8 +2017,8 @@
         <v>36</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A15),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2396243-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A15),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2396243-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2026,8 +2026,8 @@
         <v>103</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A16),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;BD &amp;amp; Mangas&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2095,8 +2095,8 @@
         <v>39</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A24),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2431293-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A24),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2431293-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2104,8 +2104,8 @@
         <v>103</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A25),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;BD &amp;amp; Mangas&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2173,8 +2173,8 @@
         <v>41</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A33),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2429939-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A33),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2429939-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2182,8 +2182,8 @@
         <v>103</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A34),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;BD &amp;amp; Mangas&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2251,8 +2251,8 @@
         <v>43</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A42),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;973074-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A42),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;973074-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2260,8 +2260,8 @@
         <v>103</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A43),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;BD &amp;amp; Mangas&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2287,8 +2287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42:I43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2343,8 +2343,8 @@
         <v>64</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A6),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2424906-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A6),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2424906-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2352,8 +2352,8 @@
         <v>62</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A7),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Science-fiction&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A7),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2421,8 +2421,8 @@
         <v>66</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A15),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2415587-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A15),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2415587-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2430,8 +2430,8 @@
         <v>62</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A16),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Science-fiction&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2499,8 +2499,8 @@
         <v>69</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A24),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2416842-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A24),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2416842-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2508,8 +2508,8 @@
         <v>62</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A25),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Science-fiction&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2577,8 +2577,8 @@
         <v>72</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A33),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2419824-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A33),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2419824-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2586,8 +2586,8 @@
         <v>62</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A34),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Science-fiction&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2655,8 +2655,8 @@
         <v>74</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A42),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;2393752-gf.jpg&lt;/categorie&gt;</v>
+        <f>CONCATENATE("&lt;image&gt;",TRIM(A42),"&lt;/image&gt;")</f>
+        <v>&lt;image&gt;2393752-gf.jpg&lt;/image&gt;</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2664,8 +2664,8 @@
         <v>62</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE("&lt;image&gt;",TRIM(A43),"&lt;/image&gt;")</f>
-        <v>&lt;image&gt;Science-fiction&lt;/image&gt;</v>
+        <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
+        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Maj XML, Panier fonctionnel, choix catégories fonctionnel
</commit_message>
<xml_diff>
--- a/WORK/Livres.xlsx
+++ b/WORK/Livres.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20010" windowHeight="12180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20010" windowHeight="12180" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
     <sheet name="Feuil4" sheetId="4" r:id="rId4"/>
     <sheet name="Feuil6" sheetId="6" r:id="rId5"/>
+    <sheet name="TOUT" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="108">
   <si>
     <t>La Disparition de Stephanie Mailer</t>
   </si>
@@ -216,9 +217,6 @@
     <t>Lucy, jeune magicienne, rêve de rejoindre la fameuse guilde de magiciens, la Fairy Tail.</t>
   </si>
   <si>
-    <t>Science-fiction</t>
-  </si>
-  <si>
     <t>Sleeping beauties</t>
   </si>
   <si>
@@ -261,88 +259,100 @@
     <t>&lt;/livre&gt;</t>
   </si>
   <si>
-    <t>JOËL DICKER</t>
-  </si>
-  <si>
-    <t>ELENA FERRANTE</t>
-  </si>
-  <si>
     <t>A la fin des années 1960, alors que les évènements de 1968 s'annoncent et que les mouvements féministes et protestataires s'organisent.</t>
   </si>
   <si>
-    <t>PIERRE LEMAITRE</t>
-  </si>
-  <si>
-    <t>JEAN D' ORMESSON</t>
-  </si>
-  <si>
-    <t>COLLECTIF</t>
-  </si>
-  <si>
-    <t>JEAN-BENOÎT NADEAU</t>
-  </si>
-  <si>
-    <t>MÉLANIE GRÉGOIRE</t>
-  </si>
-  <si>
-    <t>GUY BAILLARGEON, BRUNO RAKO</t>
-  </si>
-  <si>
-    <t>GRANT CARDONE</t>
-  </si>
-  <si>
-    <t>LAURENCE REES</t>
-  </si>
-  <si>
-    <t>KATE CLIFFORD LARSON</t>
-  </si>
-  <si>
-    <t>HENRI DORION</t>
-  </si>
-  <si>
-    <t>SARAH BAKEWELL</t>
-  </si>
-  <si>
-    <t>KEN SETTERINGTON</t>
-  </si>
-  <si>
-    <t>JARRETT J KROSOCZKA</t>
-  </si>
-  <si>
-    <t>AKIRA TORIYAMA, TOYOTARO</t>
-  </si>
-  <si>
-    <t>BEN CLANTON</t>
-  </si>
-  <si>
-    <t>HIRO MASHIMA</t>
-  </si>
-  <si>
-    <t>OWEN KING, STEPHEN KING</t>
-  </si>
-  <si>
     <t>Dans la prison pour femmes d'une petite ville des Appalaches, les femmes sont frappées d'un état léthargique et sont enveloppées dans un cocon.</t>
   </si>
   <si>
-    <t>ANDY WEIR</t>
-  </si>
-  <si>
-    <t>ANNE ROBILLARD</t>
-  </si>
-  <si>
-    <t>PATRICK SENÉCAL</t>
-  </si>
-  <si>
     <t>Il était une fois...... Alice, une jeune fille curieuse, délurée, fonceuse et intelligente de Brossard.</t>
   </si>
   <si>
-    <t>ERNEST CLINE</t>
-  </si>
-  <si>
-    <t>BD &amp;amp; Mangas</t>
-  </si>
-  <si>
-    <t>JEAN-CHRISTOPHE DERRIEN &amp;amp; AL</t>
+    <t>Jean D' Ormesson</t>
+  </si>
+  <si>
+    <t>Pierre Lemaitre</t>
+  </si>
+  <si>
+    <t>Elena Ferrante</t>
+  </si>
+  <si>
+    <t>Joël Dicker</t>
+  </si>
+  <si>
+    <t>Collectif</t>
+  </si>
+  <si>
+    <t>Owen King, Stephen King</t>
+  </si>
+  <si>
+    <t>Jarrett J Krosoczka</t>
+  </si>
+  <si>
+    <t>Laurence Rees</t>
+  </si>
+  <si>
+    <t>Jean-Benoît Nadeau</t>
+  </si>
+  <si>
+    <t>Andy Weir</t>
+  </si>
+  <si>
+    <t>Kate Clifford Larson</t>
+  </si>
+  <si>
+    <t>Mélanie Grégoire</t>
+  </si>
+  <si>
+    <t>Anne Robillard</t>
+  </si>
+  <si>
+    <t>Akira Toriyama, Toyotaro</t>
+  </si>
+  <si>
+    <t>Henri Dorion</t>
+  </si>
+  <si>
+    <t>Patrick Senécal</t>
+  </si>
+  <si>
+    <t>Ben Clanton</t>
+  </si>
+  <si>
+    <t>Sarah Bakewell</t>
+  </si>
+  <si>
+    <t>Grant Cardone</t>
+  </si>
+  <si>
+    <t>Ernest Cline</t>
+  </si>
+  <si>
+    <t>Hiro Mashima</t>
+  </si>
+  <si>
+    <t>Ken Setterington</t>
+  </si>
+  <si>
+    <t>Guy Baillargeon</t>
+  </si>
+  <si>
+    <t>Jean-Christophe Derrien</t>
+  </si>
+  <si>
+    <t>&lt;/livres&gt;</t>
+  </si>
+  <si>
+    <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;</t>
+  </si>
+  <si>
+    <t>&lt;livres&gt;</t>
+  </si>
+  <si>
+    <t>BDManga</t>
+  </si>
+  <si>
+    <t>ScienceFiction</t>
   </si>
 </sst>
 </file>
@@ -670,19 +680,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H1" t="str">
         <f>CONCATENATE("&lt;livre id=""",A1,"""&gt;")</f>
-        <v>&lt;livre id="1"&gt;</v>
+        <v>&lt;livre id="0"&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -696,11 +706,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A3),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;JOËL DICKER&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Joël Dicker&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -750,17 +760,17 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A1+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE("&lt;livre id=""",A10,"""&gt;")</f>
-        <v>&lt;livre id="2"&gt;</v>
+        <v>&lt;livre id="1"&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -774,16 +784,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I12" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A12),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;ELENA FERRANTE&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Elena Ferrante&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I13" t="str">
         <f>CONCATENATE("&lt;desc&gt;",TRIM(A13),"&lt;/desc&gt;")</f>
@@ -809,8 +819,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
+      <c r="A16" t="str">
+        <f>A7</f>
+        <v>Roman</v>
       </c>
       <c r="I16" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
@@ -828,17 +839,17 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A10+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE("&lt;livre id=""",A19,"""&gt;")</f>
-        <v>&lt;livre id="3"&gt;</v>
+        <v>&lt;livre id="2"&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -852,11 +863,11 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="I21" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A21),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;ELENA FERRANTE&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Elena Ferrante&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -887,8 +898,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
+      <c r="A25" t="str">
+        <f>A16</f>
+        <v>Roman</v>
       </c>
       <c r="I25" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
@@ -906,17 +918,17 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A19+1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H28" t="str">
         <f>CONCATENATE("&lt;livre id=""",A28,"""&gt;")</f>
-        <v>&lt;livre id="4"&gt;</v>
+        <v>&lt;livre id="3"&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -934,7 +946,7 @@
       </c>
       <c r="I30" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A30),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;PIERRE LEMAITRE&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Pierre Lemaitre&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -965,8 +977,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>2</v>
+      <c r="A34" t="str">
+        <f>A25</f>
+        <v>Roman</v>
       </c>
       <c r="I34" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
@@ -984,17 +997,17 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A28+1</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("&lt;livre id=""",A37,"""&gt;")</f>
-        <v>&lt;livre id="5"&gt;</v>
+        <v>&lt;livre id="4"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1008,20 +1021,20 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="I39" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A39),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;Le narrateur évolue entre les époques, relatant les grandes avancées culturelles de l'humanité.&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Jean D' Ormesson&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>48</v>
       </c>
       <c r="I40" t="str">
         <f>CONCATENATE("&lt;desc&gt;",TRIM(A40),"&lt;/desc&gt;")</f>
-        <v>&lt;desc&gt;JEAN D' ORMESSON&lt;/desc&gt;</v>
+        <v>&lt;desc&gt;Le narrateur évolue entre les époques, relatant les grandes avancées culturelles de l'humanité.&lt;/desc&gt;</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -1043,8 +1056,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>2</v>
+      <c r="A43" t="str">
+        <f>A34</f>
+        <v>Roman</v>
       </c>
       <c r="I43" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
@@ -1062,7 +1076,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1076,18 +1090,18 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H1" t="str">
         <f>CONCATENATE("&lt;livre id=""",A1,"""&gt;")</f>
-        <v>&lt;livre id="6"&gt;</v>
+        <v>&lt;livre id="5"&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1101,11 +1115,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A3),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;COLLECTIF&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Collectif&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1146,26 +1160,26 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A8),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A1+1</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE("&lt;livre id=""",A10,"""&gt;")</f>
-        <v>&lt;livre id="7"&gt;</v>
+        <v>&lt;livre id="6"&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1179,11 +1193,11 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="I12" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A12),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;JEAN-BENOÎT NADEAU&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Jean-Benoît Nadeau&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1214,8 +1228,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>13</v>
+      <c r="A16" t="str">
+        <f>A7</f>
+        <v>Sciences</v>
       </c>
       <c r="I16" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
@@ -1224,26 +1239,26 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A17),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A10+1</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE("&lt;livre id=""",A19,"""&gt;")</f>
-        <v>&lt;livre id="8"&gt;</v>
+        <v>&lt;livre id="7"&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1257,11 +1272,11 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="I21" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A21),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;MÉLANIE GRÉGOIRE&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Mélanie Grégoire&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1292,8 +1307,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>13</v>
+      <c r="A25" t="str">
+        <f>A16</f>
+        <v>Sciences</v>
       </c>
       <c r="I25" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
@@ -1311,17 +1327,17 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A19+1</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" t="str">
         <f>CONCATENATE("&lt;livre id=""",A28,"""&gt;")</f>
-        <v>&lt;livre id="9"&gt;</v>
+        <v>&lt;livre id="8"&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1335,11 +1351,11 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="I30" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A30),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;GUY BAILLARGEON, BRUNO RAKO&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Guy Baillargeon&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1370,8 +1386,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>13</v>
+      <c r="A34" t="str">
+        <f>A25</f>
+        <v>Sciences</v>
       </c>
       <c r="I34" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
@@ -1389,17 +1406,17 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A28+1</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("&lt;livre id=""",A37,"""&gt;")</f>
-        <v>&lt;livre id="10"&gt;</v>
+        <v>&lt;livre id="9"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1413,11 +1430,15 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>97</v>
+      </c>
+      <c r="B39" t="str">
+        <f>PROPER(A39)</f>
+        <v>Grant Cardone</v>
       </c>
       <c r="I39" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A39),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;GRANT CARDONE&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Grant Cardone&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1448,8 +1469,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>13</v>
+      <c r="A43" t="str">
+        <f>A34</f>
+        <v>Sciences</v>
       </c>
       <c r="I43" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
@@ -1467,7 +1489,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1479,19 +1501,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" t="str">
         <f>CONCATENATE("&lt;livre id=""",A1,"""&gt;")</f>
-        <v>&lt;livre id="11"&gt;</v>
+        <v>&lt;livre id="10"&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1505,11 +1527,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A3),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;LAURENCE REES&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Laurence Rees&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1550,26 +1572,26 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A8),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A1+1</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE("&lt;livre id=""",A10,"""&gt;")</f>
-        <v>&lt;livre id="12"&gt;</v>
+        <v>&lt;livre id="11"&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1583,11 +1605,11 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I12" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A12),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;KATE CLIFFORD LARSON&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Kate Clifford Larson&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1618,8 +1640,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>44</v>
+      <c r="A16" t="str">
+        <f>A7</f>
+        <v>Histoire</v>
       </c>
       <c r="I16" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
@@ -1637,17 +1660,17 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A10+1</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE("&lt;livre id=""",A19,"""&gt;")</f>
-        <v>&lt;livre id="13"&gt;</v>
+        <v>&lt;livre id="12"&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1661,11 +1684,11 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="I21" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A21),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;HENRI DORION&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Henri Dorion&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -1696,8 +1719,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>44</v>
+      <c r="A25" t="str">
+        <f>A16</f>
+        <v>Histoire</v>
       </c>
       <c r="I25" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
@@ -1715,17 +1739,17 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A19+1</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H28" t="str">
         <f>CONCATENATE("&lt;livre id=""",A28,"""&gt;")</f>
-        <v>&lt;livre id="14"&gt;</v>
+        <v>&lt;livre id="13"&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -1739,11 +1763,11 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="I30" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A30),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;SARAH BAKEWELL&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Sarah Bakewell&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1774,8 +1798,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>44</v>
+      <c r="A34" t="str">
+        <f>A25</f>
+        <v>Histoire</v>
       </c>
       <c r="I34" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
@@ -1784,26 +1809,26 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A35),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A28+1</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("&lt;livre id=""",A37,"""&gt;")</f>
-        <v>&lt;livre id="15"&gt;</v>
+        <v>&lt;livre id="14"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -1817,11 +1842,15 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>100</v>
+      </c>
+      <c r="B39" t="str">
+        <f>PROPER(A39)</f>
+        <v>Ken Setterington</v>
       </c>
       <c r="I39" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A39),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;KEN SETTERINGTON&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Ken Setterington&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -1852,8 +1881,9 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>44</v>
+      <c r="A43" t="str">
+        <f>A34</f>
+        <v>Histoire</v>
       </c>
       <c r="I43" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
@@ -1871,7 +1901,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1883,19 +1913,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" t="str">
         <f>CONCATENATE("&lt;livre id=""",A1,"""&gt;")</f>
-        <v>&lt;livre id="16"&gt;</v>
+        <v>&lt;livre id="15"&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1909,11 +1939,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A3),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;JARRETT J KROSOCZKA&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Jarrett J Krosoczka&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1945,35 +1975,35 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I7" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A7),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A8),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A1+1</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE("&lt;livre id=""",A10,"""&gt;")</f>
-        <v>&lt;livre id="17"&gt;</v>
+        <v>&lt;livre id="16"&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1987,11 +2017,11 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I12" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A12),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;JEAN-CHRISTOPHE DERRIEN &amp;amp; AL&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Jean-Christophe Derrien&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2022,12 +2052,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>103</v>
+      <c r="A16" t="str">
+        <f>A7</f>
+        <v>BDManga</v>
       </c>
       <c r="I16" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2041,17 +2072,17 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A10+1</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE("&lt;livre id=""",A19,"""&gt;")</f>
-        <v>&lt;livre id="18"&gt;</v>
+        <v>&lt;livre id="17"&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -2065,11 +2096,11 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I21" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A21),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;AKIRA TORIYAMA, TOYOTARO&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Akira Toriyama, Toyotaro&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2100,12 +2131,13 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>103</v>
+      <c r="A25" t="str">
+        <f>A16</f>
+        <v>BDManga</v>
       </c>
       <c r="I25" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2119,17 +2151,17 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A19+1</f>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" t="str">
         <f>CONCATENATE("&lt;livre id=""",A28,"""&gt;")</f>
-        <v>&lt;livre id="19"&gt;</v>
+        <v>&lt;livre id="18"&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2143,11 +2175,11 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I30" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A30),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;BEN CLANTON&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Ben Clanton&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2178,12 +2210,13 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>103</v>
+      <c r="A34" t="str">
+        <f>A25</f>
+        <v>BDManga</v>
       </c>
       <c r="I34" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2197,17 +2230,17 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A28+1</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("&lt;livre id=""",A37,"""&gt;")</f>
-        <v>&lt;livre id="20"&gt;</v>
+        <v>&lt;livre id="19"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2221,11 +2254,15 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>95</v>
+        <v>99</v>
+      </c>
+      <c r="B39" t="str">
+        <f>PROPER(A39)</f>
+        <v>Hiro Mashima</v>
       </c>
       <c r="I39" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A39),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;HIRO MASHIMA&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Hiro Mashima&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2256,26 +2293,27 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>103</v>
+      <c r="A43" t="str">
+        <f>A34</f>
+        <v>BDManga</v>
       </c>
       <c r="I43" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;BD &amp;amp; Mangas&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A44),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2287,24 +2325,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H1" t="str">
         <f>CONCATENATE("&lt;livre id=""",A1,"""&gt;")</f>
-        <v>&lt;livre id="21"&gt;</v>
+        <v>&lt;livre id="20"&gt;</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("&lt;titre&gt;",TRIM(A2),"&lt;/titre&gt;")</f>
@@ -2313,16 +2351,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A3),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;OWEN KING, STEPHEN KING&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Owen King, Stephen King&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="I4" t="str">
         <f>CONCATENATE("&lt;desc&gt;",TRIM(A4),"&lt;/desc&gt;")</f>
@@ -2340,7 +2378,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I6" t="str">
         <f>CONCATENATE("&lt;image&gt;",TRIM(A6),"&lt;/image&gt;")</f>
@@ -2349,40 +2387,40 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="I7" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A7),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A8),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>A1+1</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" t="str">
         <f>CONCATENATE("&lt;livre id=""",A10,"""&gt;")</f>
-        <v>&lt;livre id="22"&gt;</v>
+        <v>&lt;livre id="21"&gt;</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I11" t="str">
         <f>CONCATENATE("&lt;titre&gt;",TRIM(A11),"&lt;/titre&gt;")</f>
@@ -2391,16 +2429,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="I12" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A12),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;ANDY WEIR&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Andy Weir&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I13" t="str">
         <f>CONCATENATE("&lt;desc&gt;",TRIM(A13),"&lt;/desc&gt;")</f>
@@ -2418,7 +2456,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I15" t="str">
         <f>CONCATENATE("&lt;image&gt;",TRIM(A15),"&lt;/image&gt;")</f>
@@ -2426,12 +2464,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>62</v>
+      <c r="A16" t="str">
+        <f>A7</f>
+        <v>ScienceFiction</v>
       </c>
       <c r="I16" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A16),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2445,22 +2484,22 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A10+1</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H19" t="str">
         <f>CONCATENATE("&lt;livre id=""",A19,"""&gt;")</f>
-        <v>&lt;livre id="23"&gt;</v>
+        <v>&lt;livre id="22"&gt;</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I20" t="str">
         <f>CONCATENATE("&lt;titre&gt;",TRIM(A20),"&lt;/titre&gt;")</f>
@@ -2469,16 +2508,16 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I21" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A21),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;ANNE ROBILLARD&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Anne Robillard&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I22" t="str">
         <f>CONCATENATE("&lt;desc&gt;",TRIM(A22),"&lt;/desc&gt;")</f>
@@ -2496,7 +2535,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I24" t="str">
         <f>CONCATENATE("&lt;image&gt;",TRIM(A24),"&lt;/image&gt;")</f>
@@ -2504,41 +2543,42 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>62</v>
+      <c r="A25" t="str">
+        <f>A16</f>
+        <v>ScienceFiction</v>
       </c>
       <c r="I25" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A25),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26" t="str">
         <f>CONCATENATE("&lt;nouveaute&gt;",TRIM(A26),"&lt;/nouveaute&gt;")</f>
-        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A19+1</f>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H28" t="str">
         <f>CONCATENATE("&lt;livre id=""",A28,"""&gt;")</f>
-        <v>&lt;livre id="24"&gt;</v>
+        <v>&lt;livre id="23"&gt;</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I29" t="str">
         <f>CONCATENATE("&lt;titre&gt;",TRIM(A29),"&lt;/titre&gt;")</f>
@@ -2547,16 +2587,16 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="I30" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A30),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;PATRICK SENÉCAL&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Patrick Senécal&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="I31" t="str">
         <f>CONCATENATE("&lt;desc&gt;",TRIM(A31),"&lt;/desc&gt;")</f>
@@ -2574,7 +2614,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I33" t="str">
         <f>CONCATENATE("&lt;image&gt;",TRIM(A33),"&lt;/image&gt;")</f>
@@ -2582,12 +2622,13 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>62</v>
+      <c r="A34" t="str">
+        <f>A25</f>
+        <v>ScienceFiction</v>
       </c>
       <c r="I34" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A34),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2601,22 +2642,22 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H36" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>A28+1</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H37" t="str">
         <f>CONCATENATE("&lt;livre id=""",A37,"""&gt;")</f>
-        <v>&lt;livre id="25"&gt;</v>
+        <v>&lt;livre id="24"&gt;</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I38" t="str">
         <f>CONCATENATE("&lt;titre&gt;",TRIM(A38),"&lt;/titre&gt;")</f>
@@ -2625,16 +2666,20 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="B39" t="str">
+        <f>PROPER(A39)</f>
+        <v>Ernest Cline</v>
       </c>
       <c r="I39" t="str">
         <f>CONCATENATE("&lt;auteur&gt;",TRIM(A39),"&lt;/auteur&gt;")</f>
-        <v>&lt;auteur&gt;ERNEST CLINE&lt;/auteur&gt;</v>
+        <v>&lt;auteur&gt;Ernest Cline&lt;/auteur&gt;</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I40" t="str">
         <f>CONCATENATE("&lt;desc&gt;",TRIM(A40),"&lt;/desc&gt;")</f>
@@ -2652,7 +2697,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I42" t="str">
         <f>CONCATENATE("&lt;image&gt;",TRIM(A42),"&lt;/image&gt;")</f>
@@ -2660,12 +2705,13 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>62</v>
+      <c r="A43" t="str">
+        <f>A34</f>
+        <v>ScienceFiction</v>
       </c>
       <c r="I43" t="str">
         <f>CONCATENATE("&lt;categorie&gt;",TRIM(A43),"&lt;/categorie&gt;")</f>
-        <v>&lt;categorie&gt;Science-fiction&lt;/categorie&gt;</v>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2679,7 +2725,1387 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H45" t="s">
-        <v>76</v>
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C228"/>
+  <sheetViews>
+    <sheetView topLeftCell="A210" workbookViewId="0">
+      <selection sqref="A1:C228"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="str">
+        <f>Feuil1!H1</f>
+        <v>&lt;livre id="0"&gt;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="str">
+        <f>Feuil1!I2</f>
+        <v>&lt;titre&gt;La Disparition de Stephanie Mailer&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="str">
+        <f>Feuil1!I3</f>
+        <v>&lt;auteur&gt;Joël Dicker&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="str">
+        <f>Feuil1!I4</f>
+        <v>&lt;desc&gt;En 1994, dans une petite station balnéaire des Hamptons, le maire, sa femme et un témoin sont assassinés.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="str">
+        <f>Feuil1!I5</f>
+        <v>&lt;prix&gt;32,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" t="str">
+        <f>Feuil1!I6</f>
+        <v>&lt;image&gt;2435107-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" t="str">
+        <f>Feuil1!I7</f>
+        <v>&lt;categorie&gt;Roman&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="str">
+        <f>Feuil1!I8</f>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="str">
+        <f>Feuil1!H9</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="str">
+        <f>Feuil1!H10</f>
+        <v>&lt;livre id="1"&gt;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="str">
+        <f>Feuil1!I11</f>
+        <v>&lt;titre&gt;Celle qui fuit et celle qui reste&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="str">
+        <f>Feuil1!I12</f>
+        <v>&lt;auteur&gt;Elena Ferrante&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="str">
+        <f>Feuil1!I13</f>
+        <v>&lt;desc&gt;A la fin des années 1960, alors que les évènements de 1968 s'annoncent et que les mouvements féministes et protestataires s'organisent.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="str">
+        <f>Feuil1!I14</f>
+        <v>&lt;prix&gt;15,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="str">
+        <f>Feuil1!I15</f>
+        <v>&lt;image&gt;2387066-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="str">
+        <f>Feuil1!I16</f>
+        <v>&lt;categorie&gt;Roman&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="str">
+        <f>Feuil1!I17</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" t="str">
+        <f>Feuil1!H18</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="str">
+        <f>Feuil1!H19</f>
+        <v>&lt;livre id="2"&gt;</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="str">
+        <f>Feuil1!I20</f>
+        <v>&lt;titre&gt;L'Enfant perdue&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="str">
+        <f>Feuil1!I21</f>
+        <v>&lt;auteur&gt;Elena Ferrante&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="str">
+        <f>Feuil1!I22</f>
+        <v>&lt;desc&gt;Elena délaisse l'éducation de ses filles et sa carrière d'écrivain au profit de sa relation passionnelle avec Nino.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="str">
+        <f>Feuil1!I23</f>
+        <v>&lt;prix&gt;39,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="str">
+        <f>Feuil1!I24</f>
+        <v>&lt;image&gt;2387062-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="str">
+        <f>Feuil1!I25</f>
+        <v>&lt;categorie&gt;Roman&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="str">
+        <f>Feuil1!I26</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f>Feuil1!H27</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" t="str">
+        <f>Feuil1!H28</f>
+        <v>&lt;livre id="3"&gt;</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="str">
+        <f>Feuil1!I29</f>
+        <v>&lt;titre&gt;Couleurs de l'incendie&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="str">
+        <f>Feuil1!I30</f>
+        <v>&lt;auteur&gt;Pierre Lemaitre&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="str">
+        <f>Feuil1!I31</f>
+        <v>&lt;desc&gt;Second volet de la trilogie ouverte avec Au revoir là-haut.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="str">
+        <f>Feuil1!I32</f>
+        <v>&lt;prix&gt;34,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="str">
+        <f>Feuil1!I33</f>
+        <v>&lt;image&gt;2372356-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C36" t="str">
+        <f>Feuil1!I34</f>
+        <v>&lt;categorie&gt;Roman&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C37" t="str">
+        <f>Feuil1!I35</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" t="str">
+        <f>Feuil1!H36</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" t="str">
+        <f>Feuil1!H37</f>
+        <v>&lt;livre id="4"&gt;</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C40" t="str">
+        <f>Feuil1!I38</f>
+        <v>&lt;titre&gt;Et moi, je vis toujours&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C41" t="str">
+        <f>Feuil1!I39</f>
+        <v>&lt;auteur&gt;Jean D' Ormesson&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C42" t="str">
+        <f>Feuil1!I40</f>
+        <v>&lt;desc&gt;Le narrateur évolue entre les époques, relatant les grandes avancées culturelles de l'humanité.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C43" t="str">
+        <f>Feuil1!I41</f>
+        <v>&lt;prix&gt;29,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C44" t="str">
+        <f>Feuil1!I42</f>
+        <v>&lt;image&gt;2415723-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C45" t="str">
+        <f>Feuil1!I43</f>
+        <v>&lt;categorie&gt;Roman&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C46" t="str">
+        <f>Feuil1!I44</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" t="str">
+        <f>Feuil1!H45</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" t="str">
+        <f>Feuil2!H1</f>
+        <v>&lt;livre id="5"&gt;</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C49" t="str">
+        <f>Feuil2!I2</f>
+        <v>&lt;titre&gt;99 trucs pour s'enrichir&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C50" t="str">
+        <f>Feuil2!I3</f>
+        <v>&lt;auteur&gt;Collectif&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="str">
+        <f>Feuil2!I4</f>
+        <v>&lt;desc&gt;Forts du succès de la première édition, les chroniqueurs experts de la chronique « Dans vos poches » du Journal de Montréal récidivent.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C52" t="str">
+        <f>Feuil2!I5</f>
+        <v>&lt;prix&gt;19,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C53" t="str">
+        <f>Feuil2!I6</f>
+        <v>&lt;image&gt;2372509-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C54" t="str">
+        <f>Feuil2!I7</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C55" t="str">
+        <f>Feuil2!I8</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="str">
+        <f>Feuil2!H9</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="str">
+        <f>Feuil2!H10</f>
+        <v>&lt;livre id="6"&gt;</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C58" t="str">
+        <f>Feuil2!I11</f>
+        <v>&lt;titre&gt;Le Guide de la rénovation heureuse&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C59" t="str">
+        <f>Feuil2!I12</f>
+        <v>&lt;auteur&gt;Jean-Benoît Nadeau&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C60" t="str">
+        <f>Feuil2!I13</f>
+        <v>&lt;desc&gt;Après plusieurs projets personnels de rénovation, le journaliste Jean-Benoît Nadeau a réalisé un premier reportage sur ce sujet.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C61" t="str">
+        <f>Feuil2!I14</f>
+        <v>&lt;prix&gt;22,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C62" t="str">
+        <f>Feuil2!I15</f>
+        <v>&lt;image&gt;2385277-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C63" t="str">
+        <f>Feuil2!I16</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C64" t="str">
+        <f>Feuil2!I17</f>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" t="str">
+        <f>Feuil2!H18</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" t="str">
+        <f>Feuil2!H19</f>
+        <v>&lt;livre id="7"&gt;</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C67" t="str">
+        <f>Feuil2!I20</f>
+        <v>&lt;titre&gt;Les Quatre saisons de votre potager&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C68" t="str">
+        <f>Feuil2!I21</f>
+        <v>&lt;auteur&gt;Mélanie Grégoire&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C69" t="str">
+        <f>Feuil2!I22</f>
+        <v>&lt;desc&gt;Oui, la culture de vos propres légumes peut être facile et fructueuse !&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C70" t="str">
+        <f>Feuil2!I23</f>
+        <v>&lt;prix&gt;29,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C71" t="str">
+        <f>Feuil2!I24</f>
+        <v>&lt;image&gt;2420464-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C72" t="str">
+        <f>Feuil2!I25</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C73" t="str">
+        <f>Feuil2!I26</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" t="str">
+        <f>Feuil2!H27</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" t="str">
+        <f>Feuil2!H28</f>
+        <v>&lt;livre id="8"&gt;</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C76" t="str">
+        <f>Feuil2!I29</f>
+        <v>&lt;titre&gt;107 principes pour investir dans l'immobilier au québec&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C77" t="str">
+        <f>Feuil2!I30</f>
+        <v>&lt;auteur&gt;Guy Baillargeon&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C78" t="str">
+        <f>Feuil2!I31</f>
+        <v>&lt;desc&gt;Des conseils pour investir dans l'immobilier au Canada en s'adaptant aux particularités juridiques de ce marché.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="str">
+        <f>Feuil2!I32</f>
+        <v>&lt;prix&gt;29,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C80" t="str">
+        <f>Feuil2!I33</f>
+        <v>&lt;image&gt;2425434-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="str">
+        <f>Feuil2!I34</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C82" t="str">
+        <f>Feuil2!I35</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83" t="str">
+        <f>Feuil2!H36</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84" t="str">
+        <f>Feuil2!H37</f>
+        <v>&lt;livre id="9"&gt;</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C85" t="str">
+        <f>Feuil2!I38</f>
+        <v>&lt;titre&gt;Quand obsession rime avec passion&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C86" t="str">
+        <f>Feuil2!I39</f>
+        <v>&lt;auteur&gt;Grant Cardone&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C87" t="str">
+        <f>Feuil2!I40</f>
+        <v>&lt;desc&gt;L'obsession m'a sauvé la vie et a fait de moi une superstar dans le monde des affaires. que peut-elle faire pour vous ?&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C88" t="str">
+        <f>Feuil2!I41</f>
+        <v>&lt;prix&gt;24,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C89" t="str">
+        <f>Feuil2!I42</f>
+        <v>&lt;image&gt;2386203-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C90" t="str">
+        <f>Feuil2!I43</f>
+        <v>&lt;categorie&gt;Sciences&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C91" t="str">
+        <f>Feuil2!I44</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="str">
+        <f>Feuil2!H45</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93" t="str">
+        <f>Feuil3!H1</f>
+        <v>&lt;livre id="10"&gt;</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C94" t="str">
+        <f>Feuil3!I2</f>
+        <v>&lt;titre&gt;Holocauste : une nouvelle histoire&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C95" t="str">
+        <f>Feuil3!I3</f>
+        <v>&lt;auteur&gt;Laurence Rees&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C96" t="str">
+        <f>Feuil3!I4</f>
+        <v>&lt;desc&gt;Un nouvel éclairage sur la Shoah fondé sur de nombreux témoignages inédits, de documents d'époque et de travaux d'historiens.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C97" t="str">
+        <f>Feuil3!I5</f>
+        <v>&lt;prix&gt;36,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C98" t="str">
+        <f>Feuil3!I6</f>
+        <v>&lt;image&gt;2373231-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C99" t="str">
+        <f>Feuil3!I7</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C100" t="str">
+        <f>Feuil3!I8</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" t="str">
+        <f>Feuil3!H9</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" t="str">
+        <f>Feuil3!H10</f>
+        <v>&lt;livre id="11"&gt;</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C103" t="str">
+        <f>Feuil3!I11</f>
+        <v>&lt;titre&gt;Rosemary, l'enfant que l'on cachait&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C104" t="str">
+        <f>Feuil3!I12</f>
+        <v>&lt;auteur&gt;Kate Clifford Larson&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C105" t="str">
+        <f>Feuil3!I13</f>
+        <v>&lt;desc&gt;Biographie de Rosemary, soeur de John Fitzgerald Kennedy.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C106" t="str">
+        <f>Feuil3!I14</f>
+        <v>&lt;prix&gt;13,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C107" t="str">
+        <f>Feuil3!I15</f>
+        <v>&lt;image&gt;2428907-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C108" t="str">
+        <f>Feuil3!I16</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C109" t="str">
+        <f>Feuil3!I17</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110" t="str">
+        <f>Feuil3!H18</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111" t="str">
+        <f>Feuil3!H19</f>
+        <v>&lt;livre id="12"&gt;</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C112" t="str">
+        <f>Feuil3!I20</f>
+        <v>&lt;titre&gt;Villes et villages du québec : 365 questions et réponses&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C113" t="str">
+        <f>Feuil3!I21</f>
+        <v>&lt;auteur&gt;Henri Dorion&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C114" t="str">
+        <f>Feuil3!I22</f>
+        <v>&lt;desc&gt;Ce livre, le premier d'une série intitulée « Le monde en questions », se veut une présentation de 365 villes et villages du Québec au moyen d'autant de questions.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C115" t="str">
+        <f>Feuil3!I23</f>
+        <v>&lt;prix&gt;24,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C116" t="str">
+        <f>Feuil3!I24</f>
+        <v>&lt;image&gt;2443637-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C117" t="str">
+        <f>Feuil3!I25</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C118" t="str">
+        <f>Feuil3!I26</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119" t="str">
+        <f>Feuil3!H27</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120" t="str">
+        <f>Feuil3!H28</f>
+        <v>&lt;livre id="13"&gt;</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C121" t="str">
+        <f>Feuil3!I29</f>
+        <v>&lt;titre&gt;Au café existentialiste : la liberté, l'être et le cocktail à l'abricot&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C122" t="str">
+        <f>Feuil3!I30</f>
+        <v>&lt;auteur&gt;Sarah Bakewell&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C123" t="str">
+        <f>Feuil3!I31</f>
+        <v>&lt;desc&gt;Paris, 1933. Trois amis sirotent un cocktail à l'abricot : Jean-Paul Sartre, Simone de Beauvoir et Raymond Aron, tout juste rentré de Berlin où il a découvert la phénoménologie.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C124" t="str">
+        <f>Feuil3!I32</f>
+        <v>&lt;prix&gt;36,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C125" t="str">
+        <f>Feuil3!I33</f>
+        <v>&lt;image&gt;2372375-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C126" t="str">
+        <f>Feuil3!I34</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C127" t="str">
+        <f>Feuil3!I35</f>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B128" t="str">
+        <f>Feuil3!H36</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B129" t="str">
+        <f>Feuil3!H37</f>
+        <v>&lt;livre id="14"&gt;</v>
+      </c>
+    </row>
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C130" t="str">
+        <f>Feuil3!I38</f>
+        <v>&lt;titre&gt;Marqués du triangle rose&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C131" t="str">
+        <f>Feuil3!I39</f>
+        <v>&lt;auteur&gt;Ken Setterington&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C132" t="str">
+        <f>Feuil3!I40</f>
+        <v>&lt;desc&gt;Avant les années 1930, l'Allemagne, en particulier sa capitale Berlin, était l'un des endroits les plus tolérants envers les homosexuels.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C133" t="str">
+        <f>Feuil3!I41</f>
+        <v>&lt;prix&gt;17,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C134" t="str">
+        <f>Feuil3!I42</f>
+        <v>&lt;image&gt;2432344-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C135" t="str">
+        <f>Feuil3!I43</f>
+        <v>&lt;categorie&gt;Histoire&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C136" t="str">
+        <f>Feuil3!I44</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="str">
+        <f>Feuil3!H45</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="str">
+        <f>Feuil4!H1</f>
+        <v>&lt;livre id="15"&gt;</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C139" t="str">
+        <f>Feuil4!I2</f>
+        <v>&lt;titre&gt;Le Sommeil de la Force #05&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C140" t="str">
+        <f>Feuil4!I3</f>
+        <v>&lt;auteur&gt;Jarrett J Krosoczka&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C141" t="str">
+        <f>Feuil4!I4</f>
+        <v>&lt;desc&gt;Victor est de retour à l'académie et sa deuxième année ne débute pas comme il l'imaginait.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C142" t="str">
+        <f>Feuil4!I5</f>
+        <v>&lt;prix&gt;11,99&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C143" t="str">
+        <f>Feuil4!I6</f>
+        <v>&lt;image&gt;2293868-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C144" t="str">
+        <f>Feuil4!I7</f>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C145" t="str">
+        <f>Feuil4!I8</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B146" t="str">
+        <f>Feuil4!H9</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B147" t="str">
+        <f>Feuil4!H10</f>
+        <v>&lt;livre id="16"&gt;</v>
+      </c>
+    </row>
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C148" t="str">
+        <f>Feuil4!I11</f>
+        <v>&lt;titre&gt;Le Mystère des pastèques perdues #01&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C149" t="str">
+        <f>Feuil4!I12</f>
+        <v>&lt;auteur&gt;Jean-Christophe Derrien&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C150" t="str">
+        <f>Feuil4!I13</f>
+        <v>&lt;desc&gt;Frigiel, son chien Fluffy et leurs amis Alice et Abel enquêtent sur la disparition de la livraison de pastèques destinées au magasin de Koreme.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C151" t="str">
+        <f>Feuil4!I14</f>
+        <v>&lt;prix&gt;17,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C152" t="str">
+        <f>Feuil4!I15</f>
+        <v>&lt;image&gt;2396243-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C153" t="str">
+        <f>Feuil4!I16</f>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C154" t="str">
+        <f>Feuil4!I17</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B155" t="str">
+        <f>Feuil4!H18</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B156" t="str">
+        <f>Feuil4!H19</f>
+        <v>&lt;livre id="17"&gt;</v>
+      </c>
+    </row>
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C157" t="str">
+        <f>Feuil4!I20</f>
+        <v>&lt;titre&gt;Dragon ball super #03&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C158" t="str">
+        <f>Feuil4!I21</f>
+        <v>&lt;auteur&gt;Akira Toriyama, Toyotaro&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C159" t="str">
+        <f>Feuil4!I22</f>
+        <v>&lt;desc&gt;Trunks est revenu une nouvelle fois du futur ! Dans son monde, un homme ressemblant à Goku trait pour trait, surnommé Goku Black, cherche à éradiquer la race humaine.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C160" t="str">
+        <f>Feuil4!I23</f>
+        <v>&lt;prix&gt;12,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C161" t="str">
+        <f>Feuil4!I24</f>
+        <v>&lt;image&gt;2431293-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C162" t="str">
+        <f>Feuil4!I25</f>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C163" t="str">
+        <f>Feuil4!I26</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B164" t="str">
+        <f>Feuil4!H27</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B165" t="str">
+        <f>Feuil4!H28</f>
+        <v>&lt;livre id="18"&gt;</v>
+      </c>
+    </row>
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C166" t="str">
+        <f>Feuil4!I29</f>
+        <v>&lt;titre&gt;Narval, licorne de mer #01&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C167" t="str">
+        <f>Feuil4!I30</f>
+        <v>&lt;auteur&gt;Ben Clanton&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C168" t="str">
+        <f>Feuil4!I31</f>
+        <v>&lt;desc&gt;Narval est une licorne de mer insouciante. Gelato est une méduse raisonnable.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C169" t="str">
+        <f>Feuil4!I32</f>
+        <v>&lt;prix&gt;10,99&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C170" t="str">
+        <f>Feuil4!I33</f>
+        <v>&lt;image&gt;2429939-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C171" t="str">
+        <f>Feuil4!I34</f>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C172" t="str">
+        <f>Feuil4!I35</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B173" t="str">
+        <f>Feuil4!H36</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B174" t="str">
+        <f>Feuil4!H37</f>
+        <v>&lt;livre id="19"&gt;</v>
+      </c>
+    </row>
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C175" t="str">
+        <f>Feuil4!I38</f>
+        <v>&lt;titre&gt;Fairy tail #01&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C176" t="str">
+        <f>Feuil4!I39</f>
+        <v>&lt;auteur&gt;Hiro Mashima&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C177" t="str">
+        <f>Feuil4!I40</f>
+        <v>&lt;desc&gt;Lucy, jeune magicienne, rêve de rejoindre la fameuse guilde de magiciens, la Fairy Tail.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C178" t="str">
+        <f>Feuil4!I41</f>
+        <v>&lt;prix&gt;5,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C179" t="str">
+        <f>Feuil4!I42</f>
+        <v>&lt;image&gt;973074-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C180" t="str">
+        <f>Feuil4!I43</f>
+        <v>&lt;categorie&gt;BDManga&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C181" t="str">
+        <f>Feuil4!I44</f>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B182" t="str">
+        <f>Feuil4!H45</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B183" t="str">
+        <f>Feuil6!H1</f>
+        <v>&lt;livre id="20"&gt;</v>
+      </c>
+    </row>
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C184" t="str">
+        <f>Feuil6!I2</f>
+        <v>&lt;titre&gt;Sleeping beauties&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C185" t="str">
+        <f>Feuil6!I3</f>
+        <v>&lt;auteur&gt;Owen King, Stephen King&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C186" t="str">
+        <f>Feuil6!I4</f>
+        <v>&lt;desc&gt;Dans la prison pour femmes d'une petite ville des Appalaches, les femmes sont frappées d'un état léthargique et sont enveloppées dans un cocon.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C187" t="str">
+        <f>Feuil6!I5</f>
+        <v>&lt;prix&gt;39,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C188" t="str">
+        <f>Feuil6!I6</f>
+        <v>&lt;image&gt;2424906-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C189" t="str">
+        <f>Feuil6!I7</f>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C190" t="str">
+        <f>Feuil6!I8</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B191" t="str">
+        <f>Feuil6!H9</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B192" t="str">
+        <f>Feuil6!H10</f>
+        <v>&lt;livre id="21"&gt;</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C193" t="str">
+        <f>Feuil6!I11</f>
+        <v>&lt;titre&gt;Artémis éd. canada&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C194" t="str">
+        <f>Feuil6!I12</f>
+        <v>&lt;auteur&gt;Andy Weir&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C195" t="str">
+        <f>Feuil6!I13</f>
+        <v>&lt;desc&gt;Le nouveau thriller d'Andy Weir, auteur du best-seller international Seul sur Mars (The Martian)&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C196" t="str">
+        <f>Feuil6!I14</f>
+        <v>&lt;prix&gt;34,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C197" t="str">
+        <f>Feuil6!I15</f>
+        <v>&lt;image&gt;2415587-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C198" t="str">
+        <f>Feuil6!I16</f>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C199" t="str">
+        <f>Feuil6!I17</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B200" t="str">
+        <f>Feuil6!H18</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B201" t="str">
+        <f>Feuil6!H19</f>
+        <v>&lt;livre id="22"&gt;</v>
+      </c>
+    </row>
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C202" t="str">
+        <f>Feuil6!I20</f>
+        <v>&lt;titre&gt;Justiciers #09&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C203" t="str">
+        <f>Feuil6!I21</f>
+        <v>&lt;auteur&gt;Anne Robillard&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C204" t="str">
+        <f>Feuil6!I22</f>
+        <v>&lt;desc&gt;Dans l'univers, il existe une multitude de mondes parallèles et entre eux s'ouvrent parfois des portails qui nous permettent d'y accéder.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C205" t="str">
+        <f>Feuil6!I23</f>
+        <v>&lt;prix&gt;24,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C206" t="str">
+        <f>Feuil6!I24</f>
+        <v>&lt;image&gt;2416842-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C207" t="str">
+        <f>Feuil6!I25</f>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C208" t="str">
+        <f>Feuil6!I26</f>
+        <v>&lt;nouveaute&gt;1&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B209" t="str">
+        <f>Feuil6!H27</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B210" t="str">
+        <f>Feuil6!H28</f>
+        <v>&lt;livre id="23"&gt;</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C211" t="str">
+        <f>Feuil6!I29</f>
+        <v>&lt;titre&gt;Aliss&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C212" t="str">
+        <f>Feuil6!I30</f>
+        <v>&lt;auteur&gt;Patrick Senécal&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C213" t="str">
+        <f>Feuil6!I31</f>
+        <v>&lt;desc&gt;Il était une fois...... Alice, une jeune fille curieuse, délurée, fonceuse et intelligente de Brossard.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C214" t="str">
+        <f>Feuil6!I32</f>
+        <v>&lt;prix&gt;27,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C215" t="str">
+        <f>Feuil6!I33</f>
+        <v>&lt;image&gt;2419824-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C216" t="str">
+        <f>Feuil6!I34</f>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C217" t="str">
+        <f>Feuil6!I35</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B218" t="str">
+        <f>Feuil6!H36</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B219" t="str">
+        <f>Feuil6!H37</f>
+        <v>&lt;livre id="24"&gt;</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C220" t="str">
+        <f>Feuil6!I38</f>
+        <v>&lt;titre&gt;Ready player one n. éd.&lt;/titre&gt;</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C221" t="str">
+        <f>Feuil6!I39</f>
+        <v>&lt;auteur&gt;Ernest Cline&lt;/auteur&gt;</v>
+      </c>
+    </row>
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C222" t="str">
+        <f>Feuil6!I40</f>
+        <v>&lt;desc&gt;La réalité étant devenue insoutenable en 2045, la plupart de l'humanité passe son temps connectée à l'OASIS, un vaste monde virtuel.&lt;/desc&gt;</v>
+      </c>
+    </row>
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C223" t="str">
+        <f>Feuil6!I41</f>
+        <v>&lt;prix&gt;27,95&lt;/prix&gt;</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C224" t="str">
+        <f>Feuil6!I42</f>
+        <v>&lt;image&gt;2393752-gf.jpg&lt;/image&gt;</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C225" t="str">
+        <f>Feuil6!I43</f>
+        <v>&lt;categorie&gt;ScienceFiction&lt;/categorie&gt;</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C226" t="str">
+        <f>Feuil6!I44</f>
+        <v>&lt;nouveaute&gt;0&lt;/nouveaute&gt;</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B227" t="str">
+        <f>Feuil6!H45</f>
+        <v>&lt;/livre&gt;</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>